<commit_message>
Fixed bug in line of thrust and fixed derivation for line of thrust.
</commit_message>
<xml_diff>
--- a/docs/input_template_lface (with dload).xlsx
+++ b/docs/input_template_lface (with dload).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/CursorProjects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7029A2-15DA-9247-AC36-569079C05578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C8E97F-8F93-5545-BF57-4908026CEA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3860" yWindow="2180" windowWidth="30020" windowHeight="24340" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
@@ -4377,7 +4377,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5100,16 +5100,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>